<commit_message>
import bom from xlsx file
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/boms.xlsx
+++ b/spec/fixtures/files/boms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A12R17_BOM" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">C84R21_BOM!$A$7:$J$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">C84R21_BOM!$A$7:$J$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -675,7 +676,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -829,10 +830,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -862,10 +859,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -992,31 +985,32 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,6 +1118,12 @@
       <c r="L2" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="M2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="O2" s="0" t="s">
         <v>24</v>
       </c>
@@ -1182,8 +1182,12 @@
       <c r="L3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="M3" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="N3" s="14" t="n">
+        <v>4</v>
+      </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="13" t="n">
@@ -1241,6 +1245,12 @@
       <c r="L4" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="M4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="Q4" s="9" t="n">
         <v>0.21</v>
       </c>
@@ -1293,6 +1303,12 @@
       <c r="L5" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="M5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="Q5" s="11" t="n">
         <v>0.27</v>
       </c>
@@ -1344,6 +1360,12 @@
       </c>
       <c r="L6" s="0" t="s">
         <v>45</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -1372,34 +1394,34 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="11" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="13" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="11" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="11" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="11" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="11" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="11" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="11" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="13" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="11" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="11" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="11" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="11" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="11" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1471,16 +1493,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="n">
+      <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="n">
+      <c r="C2" s="38" t="n">
         <v>35</v>
       </c>
-      <c r="D2" s="38" t="n">
+      <c r="D2" s="13" t="n">
         <f aca="false">B2*C2</f>
         <v>70</v>
       </c>
@@ -1518,17 +1540,17 @@
       <c r="R2" s="11" t="n">
         <v>0.14</v>
       </c>
-      <c r="S2" s="40" t="n">
+      <c r="S2" s="39" t="n">
         <f aca="false">IF(D2&lt;100,(D2*Q2),D2*R2)</f>
         <v>14.7</v>
       </c>
-      <c r="T2" s="41" t="s">
+      <c r="T2" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="U2" s="42" t="s">
+      <c r="U2" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="43" t="n">
+      <c r="V2" s="42" t="n">
         <f aca="false">IF((D2-U2 &gt; 0), D2-U2, 0)</f>
         <v>70</v>
       </c>
@@ -2535,19 +2557,19 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="n">
+    <row r="3" s="40" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="n">
         <f aca="false">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="39" t="n">
+      <c r="C3" s="38" t="n">
         <f aca="false">C2</f>
         <v>35</v>
       </c>
-      <c r="D3" s="38" t="n">
+      <c r="D3" s="13" t="n">
         <f aca="false">B3*C3</f>
         <v>105</v>
       </c>
@@ -2579,37 +2601,37 @@
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
-      <c r="Q3" s="39" t="n">
+      <c r="Q3" s="38" t="n">
         <v>0.23</v>
       </c>
-      <c r="R3" s="39" t="n">
+      <c r="R3" s="38" t="n">
         <v>0.16</v>
       </c>
-      <c r="S3" s="44" t="n">
+      <c r="S3" s="43" t="n">
         <f aca="false">IF(D3&lt;100,(D3*Q3),D3*R3)</f>
         <v>16.8</v>
       </c>
-      <c r="U3" s="42" t="s">
+      <c r="U3" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="V3" s="43" t="n">
+      <c r="V3" s="42" t="n">
         <f aca="false">IF((D3-U3 &gt; 0), D3-U3, 0)</f>
         <v>46</v>
       </c>
     </row>
     <row r="4" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38" t="n">
+      <c r="A4" s="13" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="39" t="n">
+      <c r="C4" s="38" t="n">
         <f aca="false">C3</f>
         <v>35</v>
       </c>
-      <c r="D4" s="38" t="n">
+      <c r="D4" s="13" t="n">
         <f aca="false">B4*C4</f>
         <v>70</v>
       </c>
@@ -2643,31 +2665,31 @@
       <c r="R4" s="11" t="n">
         <v>0.2</v>
       </c>
-      <c r="S4" s="40" t="n">
+      <c r="S4" s="39" t="n">
         <f aca="false">IF(D4&lt;100,(D4*Q4),D4*R4)</f>
         <v>15.4</v>
       </c>
-      <c r="U4" s="42" t="s">
+      <c r="U4" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="V4" s="43" t="n">
+      <c r="V4" s="42" t="n">
         <f aca="false">IF((D4-U4 &gt; 0), D4-U4, 0)</f>
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="38" t="n">
+      <c r="A5" s="13" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="38" t="n">
         <f aca="false">C4</f>
         <v>35</v>
       </c>
-      <c r="D5" s="38" t="n">
+      <c r="D5" s="13" t="n">
         <f aca="false">B5*C5</f>
         <v>70</v>
       </c>
@@ -2705,15 +2727,15 @@
       <c r="R5" s="0" t="n">
         <v>0.178</v>
       </c>
-      <c r="S5" s="40" t="n">
+      <c r="S5" s="39" t="n">
         <f aca="false">IF(D5&lt;100,(D5*Q5),D5*R5)</f>
         <v>23.8</v>
       </c>
       <c r="T5" s="0"/>
-      <c r="U5" s="42" t="s">
+      <c r="U5" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="V5" s="43" t="n">
+      <c r="V5" s="42" t="n">
         <f aca="false">IF((D5-U5 &gt; 0), D5-U5, 0)</f>
         <v>28</v>
       </c>
@@ -3721,18 +3743,18 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38" t="n">
+      <c r="A6" s="13" t="n">
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="39" t="n">
+      <c r="C6" s="38" t="n">
         <f aca="false">C5</f>
         <v>35</v>
       </c>
-      <c r="D6" s="38" t="n">
+      <c r="D6" s="13" t="n">
         <f aca="false">B6*C6</f>
         <v>210</v>
       </c>
@@ -3770,15 +3792,15 @@
       <c r="R6" s="11" t="n">
         <v>0.275</v>
       </c>
-      <c r="S6" s="40" t="n">
+      <c r="S6" s="39" t="n">
         <f aca="false">IF(D6&lt;100,(D6*Q6),D6*R6)</f>
         <v>57.75</v>
       </c>
       <c r="T6" s="0"/>
-      <c r="U6" s="42" t="s">
+      <c r="U6" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="V6" s="43" t="n">
+      <c r="V6" s="42" t="n">
         <f aca="false">IF((D6-U6 &gt; 0), D6-U6, 0)</f>
         <v>136</v>
       </c>
@@ -4804,37 +4826,37 @@
   <dimension ref="1:36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="45" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="48" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="50" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="50" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="51" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="48" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="48" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="48" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="48" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="48" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="52" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="53" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="53" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="54" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="45" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="55" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="50" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="46" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="46" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="47" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="48" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="48" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="49" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="46" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="46" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="46" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="46" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="46" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="50" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="51" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="51" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="52" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="44" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="53" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="48" width="8.77551020408163"/>
   </cols>
   <sheetData>
-    <row r="1" s="61" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="59" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4883,40 +4905,40 @@
       <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="V1" s="60" t="s">
+      <c r="V1" s="58" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="n">
+      <c r="A2" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="n">
+      <c r="B2" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="47" t="n">
+      <c r="C2" s="44" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="63" t="n">
+      <c r="D2" s="61" t="n">
         <f aca="false">B2*C2</f>
         <v>60</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="48" t="s">
         <v>147</v>
       </c>
       <c r="F2" s="12" t="s">
@@ -4937,29 +4959,29 @@
       <c r="K2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="64" t="s">
+      <c r="L2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="66" t="n">
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="64" t="n">
         <v>0.1803</v>
       </c>
-      <c r="S2" s="67" t="e">
+      <c r="S2" s="65" t="e">
         <f aca="false">IF(D2&lt;100,IF(D2&lt;50,IF(D2&lt;25,D2*Q2,D2*#REF!),D2*#REF!),D2*R2)</f>
         <v>#REF!</v>
       </c>
-      <c r="T2" s="54" t="n">
+      <c r="T2" s="52" t="n">
         <v>16</v>
       </c>
-      <c r="U2" s="68" t="n">
+      <c r="U2" s="66" t="n">
         <f aca="false">IF(D2-T2 &gt; 0, D2-T2, 0)</f>
         <v>44</v>
       </c>
-      <c r="V2" s="50" t="s">
+      <c r="V2" s="48" t="s">
         <v>149</v>
       </c>
       <c r="W2" s="0"/>
@@ -5966,22 +5988,22 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="n">
+      <c r="A3" s="44" t="n">
         <f aca="false">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="62" t="n">
+      <c r="B3" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="47" t="n">
+      <c r="C3" s="44" t="n">
         <f aca="false">C2</f>
         <v>15</v>
       </c>
-      <c r="D3" s="63" t="n">
+      <c r="D3" s="61" t="n">
         <f aca="false">B3*C3</f>
         <v>15</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="46" t="s">
         <v>150</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -6009,20 +6031,20 @@
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
-      <c r="Q3" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="66" t="n">
+      <c r="Q3" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="64" t="n">
         <v>0.1803</v>
       </c>
-      <c r="S3" s="67" t="e">
+      <c r="S3" s="65" t="e">
         <f aca="false">IF(D3&lt;100,IF(D3&lt;50,IF(D3&lt;25,D3*Q3,D3*#REF!),D3*#REF!),D3*R3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="T3" s="54" t="n">
+      <c r="T3" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="U3" s="68" t="n">
+      <c r="U3" s="66" t="n">
         <f aca="false">IF(D3-T3 &gt; 0, D3-T3, 0)</f>
         <v>11</v>
       </c>
@@ -7031,40 +7053,40 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="n">
+      <c r="A4" s="44" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="62" t="n">
+      <c r="B4" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="47" t="n">
+      <c r="C4" s="44" t="n">
         <f aca="false">C3</f>
         <v>15</v>
       </c>
-      <c r="D4" s="63" t="n">
+      <c r="D4" s="61" t="n">
         <f aca="false">B4*C4</f>
         <v>15</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="47" t="s">
         <v>154</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="67" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="K4" s="70" t="s">
+      <c r="K4" s="68" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="0" t="s">
@@ -7074,20 +7096,20 @@
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
       <c r="P4" s="0"/>
-      <c r="Q4" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" s="66" t="n">
+      <c r="Q4" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="64" t="n">
         <v>0.14</v>
       </c>
-      <c r="S4" s="67" t="e">
+      <c r="S4" s="65" t="e">
         <f aca="false">IF(D4&lt;100,IF(D4&lt;50,IF(D4&lt;25,D4*Q4,D4*#REF!),D4*#REF!),D4*R4)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="T4" s="54" t="n">
+      <c r="T4" s="52" t="n">
         <v>36</v>
       </c>
-      <c r="U4" s="68" t="n">
+      <c r="U4" s="66" t="n">
         <f aca="false">IF(D4-T4 &gt; 0, D4-T4, 0)</f>
         <v>0</v>
       </c>
@@ -8096,40 +8118,40 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="n">
+      <c r="A5" s="44" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="62" t="n">
+      <c r="B5" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="47" t="n">
+      <c r="C5" s="44" t="n">
         <f aca="false">C4</f>
         <v>15</v>
       </c>
-      <c r="D5" s="63" t="n">
+      <c r="D5" s="61" t="n">
         <f aca="false">B5*C5</f>
         <v>15</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="53" t="s">
         <v>158</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="67" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="70" t="s">
+      <c r="K5" s="68" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="0" t="s">
@@ -8139,20 +8161,20 @@
       <c r="N5" s="0"/>
       <c r="O5" s="0"/>
       <c r="P5" s="0"/>
-      <c r="Q5" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="R5" s="66" t="n">
+      <c r="Q5" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" s="64" t="n">
         <v>0.2015</v>
       </c>
-      <c r="S5" s="67" t="e">
+      <c r="S5" s="65" t="e">
         <f aca="false">IF(D5&lt;100,IF(D5&lt;50,IF(D5&lt;25,D5*Q5,D5*#REF!),D5*#REF!),D5*R5)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="T5" s="54" t="n">
+      <c r="T5" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="U5" s="68" t="n">
+      <c r="U5" s="66" t="n">
         <f aca="false">IF(D5-T5 &gt; 0, D5-T5, 0)</f>
         <v>11</v>
       </c>
@@ -9161,22 +9183,22 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="n">
+      <c r="A6" s="44" t="n">
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="62" t="n">
+      <c r="B6" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="47" t="n">
+      <c r="C6" s="44" t="n">
         <f aca="false">C5</f>
         <v>15</v>
       </c>
-      <c r="D6" s="63" t="n">
+      <c r="D6" s="61" t="n">
         <f aca="false">B6*C6</f>
         <v>15</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="46" t="s">
         <v>160</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -9204,20 +9226,20 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
-      <c r="Q6" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" s="66" t="n">
+      <c r="Q6" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="64" t="n">
         <v>0.2415</v>
       </c>
-      <c r="S6" s="67" t="e">
+      <c r="S6" s="65" t="e">
         <f aca="false">IF(D6&lt;100,IF(D6&lt;50,IF(D6&lt;25,D6*Q6,D6*#REF!),D6*#REF!),D6*R6)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="T6" s="54" t="n">
+      <c r="T6" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="U6" s="68" t="n">
+      <c r="U6" s="66" t="n">
         <f aca="false">IF(D6-T6 &gt; 0, D6-T6, 0)</f>
         <v>11</v>
       </c>
@@ -10226,1592 +10248,1592 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U7" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V7" s="55" t="s">
+      <c r="A7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T7" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S8" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U8" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V8" s="55" t="s">
+      <c r="A8" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S8" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T8" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U8" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V8" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q9" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R9" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S9" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U9" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V9" s="55" t="s">
+      <c r="A9" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S9" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T9" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U9" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q10" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R10" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S10" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U10" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V10" s="55" t="s">
+      <c r="A10" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S10" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U10" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q11" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R11" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S11" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T11" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U11" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V11" s="55" t="s">
+      <c r="A11" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q11" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T11" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U11" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q12" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R12" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S12" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V12" s="55" t="s">
+      <c r="A12" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T12" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q13" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R13" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S13" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U13" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V13" s="55" t="s">
+      <c r="A13" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R14" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S14" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T14" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U14" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V14" s="55" t="s">
+      <c r="A14" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T14" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q15" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R15" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S15" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T15" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U15" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V15" s="55" t="s">
+      <c r="A15" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S15" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q16" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R16" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S16" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T16" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U16" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V16" s="55" t="s">
+      <c r="A16" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K17" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L17" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q17" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R17" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S17" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T17" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U17" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V17" s="55" t="s">
+      <c r="A17" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T17" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q18" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R18" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S18" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T18" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U18" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V18" s="55" t="s">
+      <c r="A18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q18" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S18" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T18" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V18" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q19" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R19" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S19" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T19" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U19" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V19" s="55" t="s">
+      <c r="A19" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q19" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S19" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T19" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U19" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V19" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q20" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R20" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S20" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T20" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U20" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V20" s="55" t="s">
+      <c r="A20" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S20" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T20" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U20" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q21" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R21" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S21" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T21" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U21" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V21" s="55" t="s">
+      <c r="A21" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q21" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S21" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T21" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U21" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V21" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q22" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R22" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S22" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T22" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U22" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V22" s="55" t="s">
+      <c r="A22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q22" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R22" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S22" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T22" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V22" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K23" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q23" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R23" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S23" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T23" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U23" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V23" s="55" t="s">
+      <c r="A23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K23" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L23" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q23" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R23" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S23" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T23" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V23" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q24" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R24" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S24" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T24" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U24" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V24" s="55" t="s">
+      <c r="A24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q24" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R24" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S24" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T24" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I25" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L25" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q25" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R25" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S25" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T25" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U25" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V25" s="55" t="s">
+      <c r="A25" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q25" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R25" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S25" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T25" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U25" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V25" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q26" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R26" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S26" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T26" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U26" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V26" s="55" t="s">
+      <c r="A26" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q26" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R26" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S26" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T26" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U26" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V26" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K27" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L27" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q27" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R27" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S27" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T27" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U27" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V27" s="55" t="s">
+      <c r="A27" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q27" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R27" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S27" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T27" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U27" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V27" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q28" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R28" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S28" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T28" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U28" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V28" s="55" t="s">
+      <c r="A28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q28" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S28" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T28" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V28" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J29" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K29" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q29" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R29" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S29" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T29" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U29" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V29" s="55" t="s">
+      <c r="A29" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q29" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R29" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S29" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T29" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U29" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V29" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I30" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K30" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q30" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R30" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S30" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T30" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U30" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V30" s="55" t="s">
+      <c r="A30" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L30" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q30" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R30" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S30" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T30" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U30" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V30" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K31" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L31" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q31" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R31" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S31" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T31" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U31" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V31" s="55" t="s">
+      <c r="A31" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q31" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R31" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S31" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T31" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U31" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V31" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J32" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K32" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L32" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q32" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R32" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S32" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T32" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U32" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V32" s="55" t="s">
+      <c r="A32" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I32" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q32" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R32" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S32" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T32" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U32" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V32" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J33" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K33" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L33" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q33" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R33" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S33" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T33" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U33" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V33" s="55" t="s">
+      <c r="A33" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L33" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q33" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R33" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S33" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T33" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U33" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V33" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I34" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J34" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K34" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L34" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q34" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R34" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S34" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T34" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U34" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V34" s="55" t="s">
+      <c r="A34" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J34" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K34" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L34" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q34" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R34" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S34" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T34" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U34" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V34" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H35" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I35" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="J35" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="K35" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="L35" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q35" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="R35" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="S35" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="T35" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U35" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V35" s="55" t="s">
+      <c r="A35" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K35" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L35" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q35" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="R35" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="S35" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="T35" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U35" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="V35" s="53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="I36" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="J36" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="K36" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="L36" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q36" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="R36" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="S36" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="T36" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="U36" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="V36" s="55" t="s">
+      <c r="A36" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="K36" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="L36" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q36" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="R36" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="S36" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="T36" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="U36" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="V36" s="53" t="s">
         <v>67</v>
       </c>
     </row>
@@ -11833,33 +11855,33 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="33" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="33" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2755102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8367346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="33" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="33" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11971,6 +11993,12 @@
       <c r="L2" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="M2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="Q2" s="10" t="n">
         <v>0.27</v>
       </c>
@@ -11979,7 +12007,7 @@
       </c>
       <c r="S2" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>167</v>
@@ -12025,6 +12053,12 @@
       <c r="L3" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="M3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="Q3" s="10" t="n">
         <v>0.21</v>
       </c>
@@ -12033,7 +12067,7 @@
       </c>
       <c r="S3" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12076,8 +12110,12 @@
       <c r="L4" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
+      <c r="M4" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="N4" s="13" t="n">
+        <v>28</v>
+      </c>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="34" t="n">
@@ -12088,7 +12126,7 @@
       </c>
       <c r="S4" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12131,8 +12169,12 @@
       <c r="L5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="M5" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="N5" s="11" t="n">
+        <v>28</v>
+      </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="10" t="n">
@@ -12143,7 +12185,7 @@
       </c>
       <c r="S5" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12186,6 +12228,12 @@
       <c r="L6" s="0" t="s">
         <v>177</v>
       </c>
+      <c r="M6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="Q6" s="10" t="n">
         <v>0.23</v>
       </c>
@@ -12194,7 +12242,7 @@
       </c>
       <c r="S6" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -12216,21 +12264,21 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.62755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12293,11 +12341,11 @@
       </c>
       <c r="H2" s="16" t="n">
         <f aca="false">A12R17_BOM!M2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I2" s="16" t="n">
         <f aca="false">A12R17_BOM!N2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12331,11 +12379,11 @@
       </c>
       <c r="H3" s="16" t="n">
         <f aca="false">A12R17_BOM!M3</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I3" s="16" t="n">
         <f aca="false">A12R17_BOM!N3</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12369,11 +12417,11 @@
       </c>
       <c r="H4" s="16" t="n">
         <f aca="false">A12R17_BOM!M4</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I4" s="16" t="n">
         <f aca="false">A12R17_BOM!N4</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12407,11 +12455,11 @@
       </c>
       <c r="H5" s="16" t="n">
         <f aca="false">A12R17_BOM!M5</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I5" s="16" t="n">
         <f aca="false">A12R17_BOM!N5</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12445,11 +12493,11 @@
       </c>
       <c r="H6" s="16" t="n">
         <f aca="false">A12R17_BOM!M6</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I6" s="16" t="n">
         <f aca="false">A12R17_BOM!N6</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -12471,15 +12519,15 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12821,30 +12869,31 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12965,7 +13014,7 @@
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U2" s="18" t="s">
         <v>64</v>
@@ -13018,7 +13067,7 @@
       </c>
       <c r="T3" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>67</v>
@@ -13071,7 +13120,7 @@
       </c>
       <c r="T4" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U4" s="0" t="s">
         <v>67</v>
@@ -13125,7 +13174,7 @@
       </c>
       <c r="T5" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13181,7 +13230,7 @@
       <c r="S6" s="9"/>
       <c r="T6" s="10" t="e">
         <f aca="false">IF(#REF!&lt;100,#REF!*#REF!,#REF!*#REF!)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U6" s="18"/>
     </row>
@@ -13204,21 +13253,21 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.62755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13459,15 +13508,15 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13613,29 +13662,29 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="15" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="15" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="15" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="15" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="27" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="28" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="15" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="15" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="15" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="15" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="15" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="15" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="13" style="15" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="27" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="28" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="15" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="15" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="15" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13979,31 +14028,31 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="33" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="33" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="33" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="33" width="6.75"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14356,31 +14405,31 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>